<commit_message>
trials of kouki code
</commit_message>
<xml_diff>
--- a/ENVIRONMENT_FROM_SCRATCH/configurations.xlsx
+++ b/ENVIRONMENT_FROM_SCRATCH/configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mprivitera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94582064-9140-4E3A-AD3E-F63862745E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C08D56-515B-48B4-A17B-10EDB991925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2085" windowWidth="21915" windowHeight="11385" xr2:uid="{DD8557D7-6381-4966-9350-BC63F5829D76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD8557D7-6381-4966-9350-BC63F5829D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -555,229 +555,74 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>0.05</v>
-      </c>
-      <c r="E3">
-        <v>0.05</v>
-      </c>
-      <c r="F3" s="1">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5</v>
-      </c>
-      <c r="L3" s="1">
-        <v>3</v>
-      </c>
-      <c r="M3" s="1">
-        <v>3</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4">
-        <f t="shared" ref="A4:A7" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.1</v>
-      </c>
-      <c r="E4">
-        <v>0.05</v>
-      </c>
-      <c r="F4" s="1">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>10</v>
-      </c>
-      <c r="K4" s="1">
-        <v>5</v>
-      </c>
-      <c r="L4" s="1">
-        <v>3</v>
-      </c>
-      <c r="M4" s="1">
-        <v>3</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0.15</v>
-      </c>
-      <c r="E5">
-        <v>0.05</v>
-      </c>
-      <c r="F5" s="1">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1">
-        <v>15</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>10</v>
-      </c>
-      <c r="K5" s="1">
-        <v>5</v>
-      </c>
-      <c r="L5" s="1">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0.2</v>
-      </c>
-      <c r="E6">
-        <v>0.05</v>
-      </c>
-      <c r="F6" s="1">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1">
-        <v>15</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1">
-        <v>5</v>
-      </c>
-      <c r="L6" s="1">
-        <v>3</v>
-      </c>
-      <c r="M6" s="1">
-        <v>3</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0.05</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>25</v>
-      </c>
-      <c r="G7" s="1">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>10</v>
-      </c>
-      <c r="K7" s="1">
-        <v>5</v>
-      </c>
-      <c r="L7" s="1">
-        <v>3</v>
-      </c>
-      <c r="M7" s="1">
-        <v>3</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14">
       <c r="B8" s="1"/>

</xml_diff>